<commit_message>
Add another batch of cards
</commit_message>
<xml_diff>
--- a/scripts/cards.xlsx
+++ b/scripts/cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\navarog\projects\finsearch\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D9C80B-1820-423E-88A4-29BD59FCC0E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D041EF1-A0C3-4477-A6E2-FADE3821867B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28670" yWindow="0" windowWidth="38600" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="286">
   <si>
     <t>id</t>
   </si>
@@ -694,6 +694,195 @@
   </si>
   <si>
     <t>(all players) [FishEgg][ArrowDown][FishLengthSmall] on each [AllPlayers]</t>
+  </si>
+  <si>
+    <t>Giant Hawkfish</t>
+  </si>
+  <si>
+    <t>Cirrhitus rivulatus</t>
+  </si>
+  <si>
+    <t>[FishHatch][SchoolFeederMove]</t>
+  </si>
+  <si>
+    <t>Named for its hawklike hunting technique, it perches on the high point of a coral reef and dives down upon prey.</t>
+  </si>
+  <si>
+    <t>Giant Manta Ray</t>
+  </si>
+  <si>
+    <t>Mohula birostris</t>
+  </si>
+  <si>
+    <t>[YoungFish][YoungFish][YoungFish]</t>
+  </si>
+  <si>
+    <t>The largest ray in the world, it has the biggest brain of any fish by volume—ten times larger than a whale shark’s.</t>
+  </si>
+  <si>
+    <t>Giant Oarfish</t>
+  </si>
+  <si>
+    <t>Regalecus glesne</t>
+  </si>
+  <si>
+    <t>(all players) [FishEgg][ArrowDown][FlipperBlue] on each [AllPlayers]</t>
+  </si>
+  <si>
+    <t>Rarely seen, the oarfish is the world’s longest bony fish. It’s believed to be the cause of sea serpent sightings.</t>
+  </si>
+  <si>
+    <t>Giant Trevally</t>
+  </si>
+  <si>
+    <t>Caranx ignobilis</t>
+  </si>
+  <si>
+    <t>The giant trevally is known to prey upon fledgling seabirds that fall into the water while learning to fly.</t>
+  </si>
+  <si>
+    <t>Gray Triggerfish</t>
+  </si>
+  <si>
+    <t>Balistes capriscus</t>
+  </si>
+  <si>
+    <t>Its first, tall dorsal spine remains erect until the smaller second spine is deflexed, triggering the first.</t>
+  </si>
+  <si>
+    <t>Great Northern Tilefish</t>
+  </si>
+  <si>
+    <t>Lopholatilus chamaeleonticeps</t>
+  </si>
+  <si>
+    <t>[FishHatch][FishHatch]</t>
+  </si>
+  <si>
+    <t>This colorful fish is known as the clown of the sea. It burrows into the sediment at the bottom of the ocean.</t>
+  </si>
+  <si>
+    <t>Great White Shark</t>
+  </si>
+  <si>
+    <t>Carcharodon carcharias</t>
+  </si>
+  <si>
+    <t>(all players) [FishEgg][ArrowDown][Predator] on each [AllPlayers]</t>
+  </si>
+  <si>
+    <t>Known by scientists as simply the “white shark,” this famous predator is, itself, occasionally preyed upon by orca whales.</t>
+  </si>
+  <si>
+    <t>Greenland Shark</t>
+  </si>
+  <si>
+    <t>Somniosus microcephalus</t>
+  </si>
+  <si>
+    <t>(all players) [FishEgg][ArrowDown][FishLengthLarge] on each [AllPlayers]</t>
+  </si>
+  <si>
+    <t>This shark currently holds the record as the longest-lived vertebrate, with an estimated lifespan of over 250 years.</t>
+  </si>
+  <si>
+    <t>Grideye Fish</t>
+  </si>
+  <si>
+    <t>Ipnops agassizii</t>
+  </si>
+  <si>
+    <t>[FishEgg][ArrowDown][PlayFishBottomRow] on each</t>
+  </si>
+  <si>
+    <t>Its eyes are flat, cornea-like, light-sensitive organs without lenses that cover most of the upper surface of the head.</t>
+  </si>
+  <si>
+    <t>Haddock</t>
+  </si>
+  <si>
+    <t>Melanogrammus aeglefinus</t>
+  </si>
+  <si>
+    <t>It lives on gravelly, sandy, and pebbly seafloors, where it feeds on small fish, worms, mollusks, and eggs.</t>
+  </si>
+  <si>
+    <t>Hogfish</t>
+  </si>
+  <si>
+    <t>Lachnolaimus maximus</t>
+  </si>
+  <si>
+    <t>[Discard][Discard][SchoolFeederMove]</t>
+  </si>
+  <si>
+    <t>Its common name comes from its long pig-like snout and how it roots around the seafloor searching for food.</t>
+  </si>
+  <si>
+    <t>Honeycomb Scaly Dragonfish</t>
+  </si>
+  <si>
+    <t>Stomias affinis</t>
+  </si>
+  <si>
+    <t>[YoungFish][SchoolFeederMove]</t>
+  </si>
+  <si>
+    <t>This fish can be found in deep waters during the day and in shallower areas at night, where it searches for food.</t>
+  </si>
+  <si>
+    <t>Humpback Anglerfish</t>
+  </si>
+  <si>
+    <t>Melanocetus johnsonii</t>
+  </si>
+  <si>
+    <t>(all players) [FishEgg][ArrowDown][PlayFishBottomRow] on each [AllPlayers]</t>
+  </si>
+  <si>
+    <t>The humpback anglerfish is more commonly found at shallower depths than other species in its genus.</t>
+  </si>
+  <si>
+    <t>Humphead Wrasse</t>
+  </si>
+  <si>
+    <t>Cheilinus undulatus</t>
+  </si>
+  <si>
+    <t>[FishEgg][ArrowDown][FlipperGreen] on each</t>
+  </si>
+  <si>
+    <t>It excavates by ejecting water to displace sand. Then it noses around for food.</t>
+  </si>
+  <si>
+    <t>Indo-Pacific Sailfish</t>
+  </si>
+  <si>
+    <t>Istiophorus platypterus</t>
+  </si>
+  <si>
+    <t>[DrawCard][DrawCard][FishHatch]</t>
+  </si>
+  <si>
+    <t>The world’s fastest swimming fish, its intricate dorsal fin, shaped like a sail, helps it to reach up to 110 km per hour.</t>
+  </si>
+  <si>
+    <t>Japanese Anchovy</t>
+  </si>
+  <si>
+    <t>Endraulis japonicus</t>
+  </si>
+  <si>
+    <t>Large schools tend to swim close to the surface during the full moon, their silver scales shimmering in the light.</t>
+  </si>
+  <si>
+    <t>Kaluga</t>
+  </si>
+  <si>
+    <t>Huso dauricus</t>
+  </si>
+  <si>
+    <t>Endangered throughout its range from overfishing, this sturgeon spends much of its life in estuaries and rivers.</t>
   </si>
 </sst>
 </file>
@@ -1045,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3187,6 +3376,36 @@
       <c r="B52" t="s">
         <v>4</v>
       </c>
+      <c r="C52" t="s">
+        <v>223</v>
+      </c>
+      <c r="D52" t="s">
+        <v>224</v>
+      </c>
+      <c r="G52">
+        <v>4</v>
+      </c>
+      <c r="I52">
+        <v>4</v>
+      </c>
+      <c r="L52">
+        <v>4</v>
+      </c>
+      <c r="M52">
+        <v>60</v>
+      </c>
+      <c r="N52" t="s">
+        <v>22</v>
+      </c>
+      <c r="O52" t="s">
+        <v>225</v>
+      </c>
+      <c r="S52">
+        <v>1</v>
+      </c>
+      <c r="V52" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A53">
@@ -3195,6 +3414,39 @@
       <c r="B53" t="s">
         <v>4</v>
       </c>
+      <c r="C53" t="s">
+        <v>227</v>
+      </c>
+      <c r="D53" t="s">
+        <v>228</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <v>5</v>
+      </c>
+      <c r="M53">
+        <v>900</v>
+      </c>
+      <c r="N53" t="s">
+        <v>22</v>
+      </c>
+      <c r="O53" t="s">
+        <v>229</v>
+      </c>
+      <c r="V53" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A54">
@@ -3203,6 +3455,42 @@
       <c r="B54" t="s">
         <v>4</v>
       </c>
+      <c r="C54" t="s">
+        <v>231</v>
+      </c>
+      <c r="D54" t="s">
+        <v>232</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="G54">
+        <v>2</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <v>1</v>
+      </c>
+      <c r="L54">
+        <v>9</v>
+      </c>
+      <c r="M54">
+        <v>1100</v>
+      </c>
+      <c r="N54" t="s">
+        <v>22</v>
+      </c>
+      <c r="O54" t="s">
+        <v>233</v>
+      </c>
+      <c r="S54">
+        <v>2</v>
+      </c>
+      <c r="V54" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A55">
@@ -3211,6 +3499,36 @@
       <c r="B55" t="s">
         <v>4</v>
       </c>
+      <c r="C55" t="s">
+        <v>235</v>
+      </c>
+      <c r="D55" t="s">
+        <v>236</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
+      </c>
+      <c r="L55">
+        <v>5</v>
+      </c>
+      <c r="M55">
+        <v>170</v>
+      </c>
+      <c r="N55" t="s">
+        <v>23</v>
+      </c>
+      <c r="O55" t="s">
+        <v>134</v>
+      </c>
+      <c r="V55" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A56">
@@ -3219,6 +3537,39 @@
       <c r="B56" t="s">
         <v>4</v>
       </c>
+      <c r="C56" t="s">
+        <v>238</v>
+      </c>
+      <c r="D56" t="s">
+        <v>239</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>2</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="L56">
+        <v>5</v>
+      </c>
+      <c r="M56">
+        <v>60</v>
+      </c>
+      <c r="N56" t="s">
+        <v>37</v>
+      </c>
+      <c r="O56" t="s">
+        <v>66</v>
+      </c>
+      <c r="U56" t="s">
+        <v>101</v>
+      </c>
+      <c r="V56" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A57">
@@ -3227,6 +3578,45 @@
       <c r="B57" t="s">
         <v>4</v>
       </c>
+      <c r="C57" t="s">
+        <v>241</v>
+      </c>
+      <c r="D57" t="s">
+        <v>242</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+      <c r="L57">
+        <v>4</v>
+      </c>
+      <c r="M57">
+        <v>125</v>
+      </c>
+      <c r="N57" t="s">
+        <v>37</v>
+      </c>
+      <c r="O57" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q57">
+        <v>1</v>
+      </c>
+      <c r="U57" t="s">
+        <v>102</v>
+      </c>
+      <c r="V57" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A58">
@@ -3235,6 +3625,45 @@
       <c r="B58" t="s">
         <v>4</v>
       </c>
+      <c r="C58" t="s">
+        <v>245</v>
+      </c>
+      <c r="D58" t="s">
+        <v>246</v>
+      </c>
+      <c r="G58">
+        <v>2</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="L58">
+        <v>10</v>
+      </c>
+      <c r="M58">
+        <v>600</v>
+      </c>
+      <c r="N58" t="s">
+        <v>22</v>
+      </c>
+      <c r="O58" t="s">
+        <v>247</v>
+      </c>
+      <c r="S58">
+        <v>2</v>
+      </c>
+      <c r="V58" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A59">
@@ -3243,6 +3672,42 @@
       <c r="B59" t="s">
         <v>4</v>
       </c>
+      <c r="C59" t="s">
+        <v>249</v>
+      </c>
+      <c r="D59" t="s">
+        <v>250</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+      <c r="K59">
+        <v>1</v>
+      </c>
+      <c r="L59">
+        <v>8</v>
+      </c>
+      <c r="M59">
+        <v>550</v>
+      </c>
+      <c r="N59" t="s">
+        <v>22</v>
+      </c>
+      <c r="O59" t="s">
+        <v>251</v>
+      </c>
+      <c r="S59">
+        <v>2</v>
+      </c>
+      <c r="V59" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A60">
@@ -3251,6 +3716,33 @@
       <c r="B60" t="s">
         <v>4</v>
       </c>
+      <c r="C60" t="s">
+        <v>253</v>
+      </c>
+      <c r="D60" t="s">
+        <v>254</v>
+      </c>
+      <c r="F60">
+        <v>2</v>
+      </c>
+      <c r="K60">
+        <v>1</v>
+      </c>
+      <c r="L60">
+        <v>3</v>
+      </c>
+      <c r="M60">
+        <v>16</v>
+      </c>
+      <c r="N60" t="s">
+        <v>22</v>
+      </c>
+      <c r="O60" t="s">
+        <v>255</v>
+      </c>
+      <c r="V60" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A61">
@@ -3259,6 +3751,39 @@
       <c r="B61" t="s">
         <v>4</v>
       </c>
+      <c r="C61" t="s">
+        <v>257</v>
+      </c>
+      <c r="D61" t="s">
+        <v>258</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <v>2</v>
+      </c>
+      <c r="I61">
+        <v>1</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+      <c r="L61">
+        <v>7</v>
+      </c>
+      <c r="M61">
+        <v>110</v>
+      </c>
+      <c r="N61" t="s">
+        <v>37</v>
+      </c>
+      <c r="O61" t="s">
+        <v>214</v>
+      </c>
+      <c r="V61" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A62">
@@ -3267,6 +3792,36 @@
       <c r="B62" t="s">
         <v>4</v>
       </c>
+      <c r="C62" t="s">
+        <v>260</v>
+      </c>
+      <c r="D62" t="s">
+        <v>261</v>
+      </c>
+      <c r="E62">
+        <v>2</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <v>1</v>
+      </c>
+      <c r="L62">
+        <v>6</v>
+      </c>
+      <c r="M62">
+        <v>90</v>
+      </c>
+      <c r="N62" t="s">
+        <v>22</v>
+      </c>
+      <c r="O62" t="s">
+        <v>262</v>
+      </c>
+      <c r="V62" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A63">
@@ -3275,6 +3830,48 @@
       <c r="B63" t="s">
         <v>4</v>
       </c>
+      <c r="C63" t="s">
+        <v>264</v>
+      </c>
+      <c r="D63" t="s">
+        <v>265</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>2</v>
+      </c>
+      <c r="I63">
+        <v>1</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
+      <c r="L63">
+        <v>4</v>
+      </c>
+      <c r="M63">
+        <v>22</v>
+      </c>
+      <c r="N63" t="s">
+        <v>23</v>
+      </c>
+      <c r="O63" t="s">
+        <v>266</v>
+      </c>
+      <c r="P63">
+        <v>1</v>
+      </c>
+      <c r="S63">
+        <v>1</v>
+      </c>
+      <c r="V63" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A64">
@@ -3283,6 +3880,42 @@
       <c r="B64" t="s">
         <v>4</v>
       </c>
+      <c r="C64" t="s">
+        <v>268</v>
+      </c>
+      <c r="D64" t="s">
+        <v>269</v>
+      </c>
+      <c r="G64">
+        <v>2</v>
+      </c>
+      <c r="J64">
+        <v>1</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+      <c r="L64">
+        <v>8</v>
+      </c>
+      <c r="M64">
+        <v>18</v>
+      </c>
+      <c r="N64" t="s">
+        <v>22</v>
+      </c>
+      <c r="O64" t="s">
+        <v>270</v>
+      </c>
+      <c r="P64">
+        <v>1</v>
+      </c>
+      <c r="S64">
+        <v>2</v>
+      </c>
+      <c r="V64" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A65">
@@ -3291,6 +3924,33 @@
       <c r="B65" t="s">
         <v>4</v>
       </c>
+      <c r="C65" t="s">
+        <v>272</v>
+      </c>
+      <c r="D65" t="s">
+        <v>273</v>
+      </c>
+      <c r="F65">
+        <v>2</v>
+      </c>
+      <c r="I65">
+        <v>1</v>
+      </c>
+      <c r="L65">
+        <v>4</v>
+      </c>
+      <c r="M65">
+        <v>225</v>
+      </c>
+      <c r="N65" t="s">
+        <v>22</v>
+      </c>
+      <c r="O65" t="s">
+        <v>274</v>
+      </c>
+      <c r="V65" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A66">
@@ -3299,6 +3959,39 @@
       <c r="B66" t="s">
         <v>4</v>
       </c>
+      <c r="C66" t="s">
+        <v>276</v>
+      </c>
+      <c r="D66" t="s">
+        <v>277</v>
+      </c>
+      <c r="E66">
+        <v>2</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="I66">
+        <v>1</v>
+      </c>
+      <c r="L66">
+        <v>7</v>
+      </c>
+      <c r="M66">
+        <v>350</v>
+      </c>
+      <c r="N66" t="s">
+        <v>22</v>
+      </c>
+      <c r="O66" t="s">
+        <v>278</v>
+      </c>
+      <c r="S66">
+        <v>1</v>
+      </c>
+      <c r="V66" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A67">
@@ -3307,6 +4000,42 @@
       <c r="B67" t="s">
         <v>4</v>
       </c>
+      <c r="C67" t="s">
+        <v>280</v>
+      </c>
+      <c r="D67" t="s">
+        <v>281</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="I67">
+        <v>1</v>
+      </c>
+      <c r="J67">
+        <v>1</v>
+      </c>
+      <c r="L67">
+        <v>3</v>
+      </c>
+      <c r="M67">
+        <v>18</v>
+      </c>
+      <c r="N67" t="s">
+        <v>37</v>
+      </c>
+      <c r="O67" t="s">
+        <v>77</v>
+      </c>
+      <c r="U67" t="s">
+        <v>100</v>
+      </c>
+      <c r="V67" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A68">
@@ -3314,6 +4043,36 @@
       </c>
       <c r="B68" t="s">
         <v>4</v>
+      </c>
+      <c r="C68" t="s">
+        <v>283</v>
+      </c>
+      <c r="D68" t="s">
+        <v>284</v>
+      </c>
+      <c r="E68">
+        <v>2</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <v>1</v>
+      </c>
+      <c r="L68">
+        <v>6</v>
+      </c>
+      <c r="M68">
+        <v>560</v>
+      </c>
+      <c r="N68" t="s">
+        <v>22</v>
+      </c>
+      <c r="O68" t="s">
+        <v>62</v>
+      </c>
+      <c r="V68" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Add extra cards and handle row ability icons
</commit_message>
<xml_diff>
--- a/scripts/cards.xlsx
+++ b/scripts/cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\navarog\projects\finsearch\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D041EF1-A0C3-4477-A6E2-FADE3821867B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3613B63A-DC28-4128-9332-1FD27C623337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28670" yWindow="0" windowWidth="38600" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28720" yWindow="0" windowWidth="38570" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="349">
   <si>
     <t>id</t>
   </si>
@@ -883,6 +883,195 @@
   </si>
   <si>
     <t>Endangered throughout its range from overfishing, this sturgeon spends much of its life in estuaries and rivers.</t>
+  </si>
+  <si>
+    <t>Kawakawa</t>
+  </si>
+  <si>
+    <t>Euthynnus affinis</t>
+  </si>
+  <si>
+    <t>[FishEgg][ArrowDown][FlipperBlue]</t>
+  </si>
+  <si>
+    <t>Adults live in open waters but remain close to the shoreline. Their young may enter bays and harbors.</t>
+  </si>
+  <si>
+    <t>Largetooth Flounder</t>
+  </si>
+  <si>
+    <t>Pseudorhombus arsius</t>
+  </si>
+  <si>
+    <t>[FishEgg][ArrowDown][FlipperGreen]</t>
+  </si>
+  <si>
+    <t>The largetooth flounder is a species of left- eyed flatfish with both eyes of the adult on the left side of its body.</t>
+  </si>
+  <si>
+    <t>Leafy Seadragon</t>
+  </si>
+  <si>
+    <t>Phycodurus eques</t>
+  </si>
+  <si>
+    <t>Lobes of skin growing all over it provide camouflage, giving it the appearance of seaweed, even as it swims.</t>
+  </si>
+  <si>
+    <t>Live Sharksucker</t>
+  </si>
+  <si>
+    <t>Echeneis naucrates</t>
+  </si>
+  <si>
+    <t>[ConsumeFish1][ConsumeFish1]</t>
+  </si>
+  <si>
+    <t>This fish can attach itself to any large host, even scuba divers, using the oval-shaped sucking disc on its head.</t>
+  </si>
+  <si>
+    <t>Long-Snouted Lancetfish</t>
+  </si>
+  <si>
+    <t>Alepisaurus ferox</t>
+  </si>
+  <si>
+    <t>[DrawCard][DrawCard][DrawCard][SchoolFeederMove]</t>
+  </si>
+  <si>
+    <t>Voracious eaters, many new species of fish and mollusks have been discovered in the contents of their stomachs.</t>
+  </si>
+  <si>
+    <t>Longspine Porcupinefish</t>
+  </si>
+  <si>
+    <t>Diodon holocanthus</t>
+  </si>
+  <si>
+    <t>It uses its beak and the plates on the roof of its mouth to crush prey that would otherwise be indigestible.</t>
+  </si>
+  <si>
+    <t>Mahi-Mahi</t>
+  </si>
+  <si>
+    <t>Coryphaena hippurus</t>
+  </si>
+  <si>
+    <t>Its common name means “strong-strong” in Hawaiian. Flyingfishes make up nearly 25% of the diet of adults.</t>
+  </si>
+  <si>
+    <t>Maletese Ray</t>
+  </si>
+  <si>
+    <t>Leucoraja melitensis</t>
+  </si>
+  <si>
+    <t>Critically endangered due to habitat loss, the Maltese ray faces a high risk of extinction in the wild.</t>
+  </si>
+  <si>
+    <t>Mariana Snailfish</t>
+  </si>
+  <si>
+    <t>Pseudoliparis swirei</t>
+  </si>
+  <si>
+    <t>It has been observed at a depth of 8,178 m, making it one of the deepest dwelling fishes on the planet.</t>
+  </si>
+  <si>
+    <t>Mediterranean Damselfish</t>
+  </si>
+  <si>
+    <t>Chromis chromis</t>
+  </si>
+  <si>
+    <t>Though normally a peaceful species, males aggressively guard the eggs while they develop.</t>
+  </si>
+  <si>
+    <t>Mediterranean Parrotfish</t>
+  </si>
+  <si>
+    <t>Sparisoma cretense</t>
+  </si>
+  <si>
+    <t>It starts life as female, then changes to male in adulthood, turning from bright red and yellow to gray and blue.</t>
+  </si>
+  <si>
+    <t>Midwater Scorpionfish</t>
+  </si>
+  <si>
+    <t>Ectreposebastes imus</t>
+  </si>
+  <si>
+    <t>This fish has often been seen suspending itself vertically in the water, with its mouth pointing up towards the surface.</t>
+  </si>
+  <si>
+    <t>Ocean sunfish</t>
+  </si>
+  <si>
+    <t>Mola mola</t>
+  </si>
+  <si>
+    <t>The largest known bony fish, it basks on the surface to thermally recharge after feeding in deeper, colder waters.</t>
+  </si>
+  <si>
+    <t>Oceanic Puffer</t>
+  </si>
+  <si>
+    <t>Lagocephalus lagocephalus</t>
+  </si>
+  <si>
+    <t>Its Latin name means “rabbit head,” and, like many puffers, it contains neurotoxins that may be fatal to humans if eaten.</t>
+  </si>
+  <si>
+    <t>Pacific Sardine</t>
+  </si>
+  <si>
+    <t>Sardinops sagax</t>
+  </si>
+  <si>
+    <t>[FishEgg][FishEgg][FishHatch][FishHatch]</t>
+  </si>
+  <si>
+    <t>Forming schools of up to 10 million fish, it is, at times, the most abundant species in the California Current.</t>
+  </si>
+  <si>
+    <t>Pacific White Skate</t>
+  </si>
+  <si>
+    <t>Bathyraja spinosissima</t>
+  </si>
+  <si>
+    <t>[FishHatch][YoungFish]</t>
+  </si>
+  <si>
+    <t>Most skates only have dermal denticles on their dorsal side, but this one has tiny spines on its belly as well.</t>
+  </si>
+  <si>
+    <t>Pale Chimaera</t>
+  </si>
+  <si>
+    <t>Hydrolagus pallidus</t>
+  </si>
+  <si>
+    <t>Dubbed “ghost sharks,” chimaeras “flap” their large pectoral fins to propel themselves forward (unlike sharks).</t>
+  </si>
+  <si>
+    <t>Paintspotted Moray</t>
+  </si>
+  <si>
+    <t>Gymnothorax pictus</t>
+  </si>
+  <si>
+    <t>[Discard][Discard][Discard]</t>
+  </si>
+  <si>
+    <t>It inhabits reef flats and rocky intertidal shorelines, and it will sometimes leave the water in pursuit of prey.</t>
+  </si>
+  <si>
+    <t>3 [Wave] if [SchoolFish] on this fish</t>
+  </si>
+  <si>
+    <t>10 [Wave] if [FishEgg] + [YoungFish] + [SchoolFish] on this fish</t>
   </si>
 </sst>
 </file>
@@ -918,9 +1107,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1234,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="O83" sqref="O83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2917,7 +3105,7 @@
       <c r="U40" t="s">
         <v>100</v>
       </c>
-      <c r="V40" s="1" t="s">
+      <c r="V40" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3383,7 +3571,7 @@
         <v>224</v>
       </c>
       <c r="G52">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I52">
         <v>4</v>
@@ -4082,6 +4270,36 @@
       <c r="B69" t="s">
         <v>4</v>
       </c>
+      <c r="C69" t="s">
+        <v>286</v>
+      </c>
+      <c r="D69" t="s">
+        <v>287</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69">
+        <v>2</v>
+      </c>
+      <c r="I69">
+        <v>1</v>
+      </c>
+      <c r="L69">
+        <v>6</v>
+      </c>
+      <c r="M69">
+        <v>100</v>
+      </c>
+      <c r="N69" t="s">
+        <v>22</v>
+      </c>
+      <c r="O69" t="s">
+        <v>288</v>
+      </c>
+      <c r="V69" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A70">
@@ -4090,6 +4308,36 @@
       <c r="B70" t="s">
         <v>4</v>
       </c>
+      <c r="C70" t="s">
+        <v>290</v>
+      </c>
+      <c r="D70" t="s">
+        <v>291</v>
+      </c>
+      <c r="E70">
+        <v>3</v>
+      </c>
+      <c r="I70">
+        <v>1</v>
+      </c>
+      <c r="L70">
+        <v>5</v>
+      </c>
+      <c r="M70">
+        <v>45</v>
+      </c>
+      <c r="N70" t="s">
+        <v>23</v>
+      </c>
+      <c r="O70" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q70">
+        <v>1</v>
+      </c>
+      <c r="V70" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A71">
@@ -4098,6 +4346,36 @@
       <c r="B71" t="s">
         <v>4</v>
       </c>
+      <c r="C71" t="s">
+        <v>294</v>
+      </c>
+      <c r="D71" t="s">
+        <v>295</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+      <c r="I71">
+        <v>1</v>
+      </c>
+      <c r="L71">
+        <v>2</v>
+      </c>
+      <c r="M71">
+        <v>35</v>
+      </c>
+      <c r="N71" t="s">
+        <v>23</v>
+      </c>
+      <c r="O71" t="s">
+        <v>347</v>
+      </c>
+      <c r="Q71">
+        <v>1</v>
+      </c>
+      <c r="V71" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A72">
@@ -4147,6 +4425,33 @@
       <c r="B73" t="s">
         <v>4</v>
       </c>
+      <c r="C73" t="s">
+        <v>297</v>
+      </c>
+      <c r="D73" t="s">
+        <v>298</v>
+      </c>
+      <c r="F73">
+        <v>2</v>
+      </c>
+      <c r="I73">
+        <v>1</v>
+      </c>
+      <c r="L73">
+        <v>4</v>
+      </c>
+      <c r="M73">
+        <v>110</v>
+      </c>
+      <c r="N73" t="s">
+        <v>22</v>
+      </c>
+      <c r="O73" t="s">
+        <v>299</v>
+      </c>
+      <c r="V73" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A74">
@@ -4155,6 +4460,42 @@
       <c r="B74" t="s">
         <v>4</v>
       </c>
+      <c r="C74" t="s">
+        <v>301</v>
+      </c>
+      <c r="D74" t="s">
+        <v>302</v>
+      </c>
+      <c r="H74">
+        <v>1</v>
+      </c>
+      <c r="I74">
+        <v>1</v>
+      </c>
+      <c r="J74">
+        <v>1</v>
+      </c>
+      <c r="K74">
+        <v>1</v>
+      </c>
+      <c r="L74">
+        <v>3</v>
+      </c>
+      <c r="M74">
+        <v>200</v>
+      </c>
+      <c r="N74" t="s">
+        <v>22</v>
+      </c>
+      <c r="O74" t="s">
+        <v>303</v>
+      </c>
+      <c r="S74">
+        <v>1</v>
+      </c>
+      <c r="V74" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A75">
@@ -4163,6 +4504,39 @@
       <c r="B75" t="s">
         <v>4</v>
       </c>
+      <c r="C75" t="s">
+        <v>305</v>
+      </c>
+      <c r="D75" t="s">
+        <v>306</v>
+      </c>
+      <c r="E75">
+        <v>2</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+      <c r="I75">
+        <v>1</v>
+      </c>
+      <c r="L75">
+        <v>5</v>
+      </c>
+      <c r="M75">
+        <v>50</v>
+      </c>
+      <c r="N75" t="s">
+        <v>22</v>
+      </c>
+      <c r="O75" t="s">
+        <v>130</v>
+      </c>
+      <c r="T75">
+        <v>1</v>
+      </c>
+      <c r="V75" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A76">
@@ -4171,6 +4545,39 @@
       <c r="B76" t="s">
         <v>4</v>
       </c>
+      <c r="C76" t="s">
+        <v>308</v>
+      </c>
+      <c r="D76" t="s">
+        <v>309</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76">
+        <v>2</v>
+      </c>
+      <c r="I76">
+        <v>1</v>
+      </c>
+      <c r="L76">
+        <v>7</v>
+      </c>
+      <c r="M76">
+        <v>210</v>
+      </c>
+      <c r="N76" t="s">
+        <v>37</v>
+      </c>
+      <c r="O76" t="s">
+        <v>77</v>
+      </c>
+      <c r="S76">
+        <v>1</v>
+      </c>
+      <c r="V76" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A77">
@@ -4179,6 +4586,39 @@
       <c r="B77" t="s">
         <v>4</v>
       </c>
+      <c r="C77" t="s">
+        <v>311</v>
+      </c>
+      <c r="D77" t="s">
+        <v>312</v>
+      </c>
+      <c r="F77">
+        <v>2</v>
+      </c>
+      <c r="I77">
+        <v>1</v>
+      </c>
+      <c r="J77">
+        <v>1</v>
+      </c>
+      <c r="L77">
+        <v>3</v>
+      </c>
+      <c r="M77">
+        <v>40</v>
+      </c>
+      <c r="N77" t="s">
+        <v>22</v>
+      </c>
+      <c r="O77" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q77">
+        <v>1</v>
+      </c>
+      <c r="V77" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A78">
@@ -4187,6 +4627,33 @@
       <c r="B78" t="s">
         <v>4</v>
       </c>
+      <c r="C78" t="s">
+        <v>314</v>
+      </c>
+      <c r="D78" t="s">
+        <v>315</v>
+      </c>
+      <c r="E78">
+        <v>2</v>
+      </c>
+      <c r="K78">
+        <v>2</v>
+      </c>
+      <c r="L78">
+        <v>1</v>
+      </c>
+      <c r="M78">
+        <v>28</v>
+      </c>
+      <c r="N78" t="s">
+        <v>23</v>
+      </c>
+      <c r="O78" t="s">
+        <v>255</v>
+      </c>
+      <c r="V78" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="79" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A79">
@@ -4195,6 +4662,36 @@
       <c r="B79" t="s">
         <v>4</v>
       </c>
+      <c r="C79" t="s">
+        <v>317</v>
+      </c>
+      <c r="D79" t="s">
+        <v>318</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="I79">
+        <v>1</v>
+      </c>
+      <c r="L79">
+        <v>4</v>
+      </c>
+      <c r="M79">
+        <v>25</v>
+      </c>
+      <c r="N79" t="s">
+        <v>37</v>
+      </c>
+      <c r="O79" t="s">
+        <v>77</v>
+      </c>
+      <c r="U79" t="s">
+        <v>100</v>
+      </c>
+      <c r="V79" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="80" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A80">
@@ -4203,64 +4700,319 @@
       <c r="B80" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C80" t="s">
+        <v>320</v>
+      </c>
+      <c r="D80" t="s">
+        <v>321</v>
+      </c>
+      <c r="E80">
+        <v>2</v>
+      </c>
+      <c r="F80">
+        <v>1</v>
+      </c>
+      <c r="I80">
+        <v>1</v>
+      </c>
+      <c r="L80">
+        <v>5</v>
+      </c>
+      <c r="M80">
+        <v>50</v>
+      </c>
+      <c r="N80" t="s">
+        <v>37</v>
+      </c>
+      <c r="O80" t="s">
+        <v>70</v>
+      </c>
+      <c r="U80" t="s">
+        <v>102</v>
+      </c>
+      <c r="V80" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="81" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C81" t="s">
+        <v>323</v>
+      </c>
+      <c r="D81" t="s">
+        <v>324</v>
+      </c>
+      <c r="E81">
+        <v>3</v>
+      </c>
+      <c r="I81">
+        <v>1</v>
+      </c>
+      <c r="J81">
+        <v>1</v>
+      </c>
+      <c r="K81">
+        <v>1</v>
+      </c>
+      <c r="L81">
+        <v>3</v>
+      </c>
+      <c r="M81">
+        <v>18</v>
+      </c>
+      <c r="N81" t="s">
+        <v>37</v>
+      </c>
+      <c r="O81" t="s">
+        <v>38</v>
+      </c>
+      <c r="T81">
+        <v>1</v>
+      </c>
+      <c r="V81" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="82" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C82" t="s">
+        <v>326</v>
+      </c>
+      <c r="D82" t="s">
+        <v>327</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="F82">
+        <v>2</v>
+      </c>
+      <c r="I82">
+        <v>1</v>
+      </c>
+      <c r="J82">
+        <v>1</v>
+      </c>
+      <c r="L82">
+        <v>4</v>
+      </c>
+      <c r="M82">
+        <v>330</v>
+      </c>
+      <c r="N82" t="s">
+        <v>23</v>
+      </c>
+      <c r="O82" t="s">
+        <v>176</v>
+      </c>
+      <c r="V82" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="83" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C83" t="s">
+        <v>329</v>
+      </c>
+      <c r="D83" t="s">
+        <v>330</v>
+      </c>
+      <c r="E83">
+        <v>2</v>
+      </c>
+      <c r="I83">
+        <v>1</v>
+      </c>
+      <c r="J83">
+        <v>1</v>
+      </c>
+      <c r="L83">
+        <v>5</v>
+      </c>
+      <c r="M83">
+        <v>60</v>
+      </c>
+      <c r="N83" t="s">
+        <v>37</v>
+      </c>
+      <c r="O83" t="s">
+        <v>215</v>
+      </c>
+      <c r="T83">
+        <v>1</v>
+      </c>
+      <c r="V83" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="84" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C84" t="s">
+        <v>332</v>
+      </c>
+      <c r="D84" t="s">
+        <v>333</v>
+      </c>
+      <c r="E84">
+        <v>3</v>
+      </c>
+      <c r="I84">
+        <v>1</v>
+      </c>
+      <c r="L84">
+        <v>4</v>
+      </c>
+      <c r="M84">
+        <v>40</v>
+      </c>
+      <c r="N84" t="s">
+        <v>22</v>
+      </c>
+      <c r="O84" t="s">
+        <v>334</v>
+      </c>
+      <c r="V84" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="85" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C85" t="s">
+        <v>336</v>
+      </c>
+      <c r="D85" t="s">
+        <v>337</v>
+      </c>
+      <c r="F85">
+        <v>2</v>
+      </c>
+      <c r="J85">
+        <v>1</v>
+      </c>
+      <c r="K85">
+        <v>1</v>
+      </c>
+      <c r="L85">
+        <v>3</v>
+      </c>
+      <c r="M85">
+        <v>150</v>
+      </c>
+      <c r="N85" t="s">
+        <v>22</v>
+      </c>
+      <c r="O85" t="s">
+        <v>338</v>
+      </c>
+      <c r="V85" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="86" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C86" t="s">
+        <v>340</v>
+      </c>
+      <c r="D86" t="s">
+        <v>341</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+      <c r="J86">
+        <v>1</v>
+      </c>
+      <c r="K86">
+        <v>1</v>
+      </c>
+      <c r="L86">
+        <v>2</v>
+      </c>
+      <c r="M86">
+        <v>137</v>
+      </c>
+      <c r="N86" t="s">
+        <v>23</v>
+      </c>
+      <c r="O86" t="s">
+        <v>348</v>
+      </c>
+      <c r="V86" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="87" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C87" t="s">
+        <v>343</v>
+      </c>
+      <c r="D87" t="s">
+        <v>344</v>
+      </c>
+      <c r="F87">
+        <v>2</v>
+      </c>
+      <c r="I87">
+        <v>1</v>
+      </c>
+      <c r="L87">
+        <v>4</v>
+      </c>
+      <c r="M87">
+        <v>140</v>
+      </c>
+      <c r="N87" t="s">
+        <v>22</v>
+      </c>
+      <c r="O87" t="s">
+        <v>345</v>
+      </c>
+      <c r="S87">
+        <v>1</v>
+      </c>
+      <c r="V87" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="88" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4268,7 +5020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4276,7 +5028,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4284,7 +5036,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4292,7 +5044,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4300,7 +5052,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4308,7 +5060,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4316,7 +5068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4324,7 +5076,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A96">
         <v>95</v>
       </c>

</xml_diff>